<commit_message>
update training and experiments
</commit_message>
<xml_diff>
--- a/data/prune24_old.xlsx
+++ b/data/prune24_old.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\tex\FPGA19\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="stage1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="269">
   <si>
     <t>2018-09-26 09</t>
   </si>
@@ -818,31 +818,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>p2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>p4</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>p5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>p6</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p7</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p8</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -863,6 +843,10 @@
   </si>
   <si>
     <t>p8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1537,7 +1521,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3553,7 +3536,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6059,7 +6041,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p1</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6452,7 +6434,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p2</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6827,7 +6809,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p3</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7184,7 +7166,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p4</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7523,7 +7505,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p5</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7844,7 +7826,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p6</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8149,7 +8131,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p7</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8436,7 +8418,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p8</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8922,7 +8904,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>top 1</c:v>
+                  <c:v>baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9309,7 +9291,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p1</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9714,7 +9696,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p2</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10101,7 +10083,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p3</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10470,7 +10452,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p4</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10821,7 +10803,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p5</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11154,7 +11136,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p6</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11475,7 +11457,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p7</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -28825,7 +28807,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K591"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
@@ -53845,8 +53827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L1" activeCellId="1" sqref="A1:A61 L1:S61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -53858,56 +53840,56 @@
       <c r="B1" t="s">
         <v>258</v>
       </c>
-      <c r="C1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F1" t="s">
-        <v>262</v>
-      </c>
-      <c r="G1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I1" t="s">
-        <v>265</v>
-      </c>
-      <c r="J1" t="s">
-        <v>266</v>
+      <c r="C1">
+        <v>30</v>
+      </c>
+      <c r="D1">
+        <v>60</v>
+      </c>
+      <c r="E1">
+        <v>90</v>
+      </c>
+      <c r="F1">
+        <v>120</v>
+      </c>
+      <c r="G1">
+        <v>150</v>
+      </c>
+      <c r="H1">
+        <v>180</v>
+      </c>
+      <c r="I1">
+        <v>210</v>
+      </c>
+      <c r="J1">
+        <v>240</v>
       </c>
       <c r="L1" t="s">
-        <v>252</v>
-      </c>
-      <c r="M1" t="s">
-        <v>259</v>
-      </c>
-      <c r="N1" t="s">
-        <v>260</v>
-      </c>
-      <c r="O1" t="s">
-        <v>261</v>
-      </c>
-      <c r="P1" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>263</v>
-      </c>
-      <c r="R1" t="s">
-        <v>264</v>
-      </c>
-      <c r="S1" t="s">
-        <v>265</v>
-      </c>
-      <c r="T1" t="s">
-        <v>266</v>
+        <v>268</v>
+      </c>
+      <c r="M1">
+        <v>30</v>
+      </c>
+      <c r="N1">
+        <v>60</v>
+      </c>
+      <c r="O1">
+        <v>90</v>
+      </c>
+      <c r="P1">
+        <v>120</v>
+      </c>
+      <c r="Q1">
+        <v>150</v>
+      </c>
+      <c r="R1">
+        <v>180</v>
+      </c>
+      <c r="S1">
+        <v>210</v>
+      </c>
+      <c r="T1">
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -56094,7 +56076,7 @@
   <dimension ref="A1:J301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -56104,31 +56086,31 @@
         <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C1" t="s">
         <v>259</v>
       </c>
       <c r="D1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="J1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>